<commit_message>
[IMP] New test data
</commit_message>
<xml_diff>
--- a/clodoo/clodoo/transodoo.xlsx
+++ b/clodoo/clodoo/transodoo.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2010" uniqueCount="783">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2014" uniqueCount="784">
   <si>
     <t xml:space="preserve">model</t>
   </si>
@@ -2294,6 +2294,9 @@
   </si>
   <si>
     <t xml:space="preserve">zip</t>
+  </si>
+  <si>
+    <t xml:space="preserve">notify_email</t>
   </si>
   <si>
     <t xml:space="preserve">res.users</t>
@@ -2378,7 +2381,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -2436,6 +2439,13 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -2479,7 +2489,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2501,6 +2511,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2584,12 +2598,12 @@
   <dimension ref="A1:Y1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="630" topLeftCell="N117" activePane="bottomLeft" state="split"/>
+      <pane xSplit="0" ySplit="630" topLeftCell="N427" activePane="bottomLeft" state="split"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A144" activeCellId="0" sqref="A144"/>
+      <selection pane="bottomLeft" activeCell="B444" activeCellId="0" sqref="B444"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="27.30078125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="27.30859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.75"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="24.3"/>
@@ -9355,115 +9369,136 @@
         <v>757</v>
       </c>
     </row>
-    <row r="449" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A449" s="1" t="s">
+    <row r="449" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A449" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="B449" s="4"/>
+      <c r="C449" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D449" s="4" t="s">
         <v>758</v>
       </c>
-      <c r="C449" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D449" s="2" t="s">
-        <v>759</v>
-      </c>
-      <c r="E449" s="1" t="s">
-        <v>760</v>
-      </c>
+      <c r="E449" s="4"/>
+      <c r="F449" s="4"/>
+      <c r="G449" s="4"/>
+      <c r="H449" s="4"/>
+      <c r="I449" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="J449" s="4"/>
+      <c r="K449" s="4"/>
+      <c r="L449" s="4"/>
+      <c r="M449" s="4"/>
+      <c r="N449" s="4"/>
+      <c r="O449" s="4"/>
+      <c r="P449" s="4"/>
+      <c r="Q449" s="4"/>
+      <c r="R449" s="4"/>
+      <c r="S449" s="4"/>
+      <c r="T449" s="4"/>
+      <c r="U449" s="4"/>
+      <c r="V449" s="4"/>
+      <c r="W449" s="4"/>
+      <c r="X449" s="4"/>
+      <c r="Y449" s="4"/>
     </row>
     <row r="450" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A450" s="1" t="s">
-        <v>758</v>
+        <v>759</v>
       </c>
       <c r="C450" s="1" t="s">
         <v>26</v>
       </c>
       <c r="D450" s="2" t="s">
+        <v>760</v>
+      </c>
+      <c r="E450" s="1" t="s">
         <v>761</v>
-      </c>
-      <c r="E450" s="1" t="s">
-        <v>762</v>
       </c>
     </row>
     <row r="451" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A451" s="1" t="s">
-        <v>758</v>
+        <v>759</v>
       </c>
       <c r="C451" s="1" t="s">
         <v>26</v>
       </c>
+      <c r="D451" s="2" t="s">
+        <v>762</v>
+      </c>
       <c r="E451" s="1" t="s">
-        <v>742</v>
+        <v>763</v>
       </c>
     </row>
     <row r="452" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A452" s="1" t="s">
-        <v>758</v>
+        <v>759</v>
       </c>
       <c r="C452" s="1" t="s">
         <v>26</v>
       </c>
       <c r="E452" s="1" t="s">
-        <v>763</v>
+        <v>742</v>
       </c>
     </row>
     <row r="453" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A453" s="1" t="s">
-        <v>758</v>
+        <v>759</v>
       </c>
       <c r="C453" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D453" s="2" t="s">
+      <c r="E453" s="1" t="s">
         <v>764</v>
-      </c>
-      <c r="E453" s="1" t="s">
-        <v>765</v>
       </c>
     </row>
     <row r="454" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A454" s="1" t="s">
+        <v>759</v>
+      </c>
+      <c r="C454" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D454" s="2" t="s">
+        <v>765</v>
+      </c>
+      <c r="E454" s="1" t="s">
         <v>766</v>
-      </c>
-      <c r="C454" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="D454" s="2" t="s">
-        <v>767</v>
-      </c>
-      <c r="G454" s="1" t="s">
-        <v>768</v>
       </c>
     </row>
     <row r="455" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A455" s="1" t="s">
-        <v>766</v>
+        <v>767</v>
       </c>
       <c r="C455" s="1" t="s">
-        <v>26</v>
+        <v>76</v>
       </c>
       <c r="D455" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="H455" s="2" t="s">
-        <v>94</v>
+        <v>768</v>
+      </c>
+      <c r="G455" s="1" t="s">
+        <v>769</v>
       </c>
     </row>
     <row r="456" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A456" s="1" t="s">
-        <v>766</v>
-      </c>
-      <c r="B456" s="2" t="s">
-        <v>123</v>
+        <v>767</v>
       </c>
       <c r="C456" s="1" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="D456" s="2" t="s">
-        <v>671</v>
+        <v>93</v>
+      </c>
+      <c r="H456" s="2" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="457" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A457" s="1" t="s">
-        <v>766</v>
+        <v>767</v>
       </c>
       <c r="B457" s="2" t="s">
         <v>123</v>
@@ -9472,12 +9507,12 @@
         <v>34</v>
       </c>
       <c r="D457" s="2" t="s">
-        <v>674</v>
+        <v>671</v>
       </c>
     </row>
     <row r="458" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A458" s="1" t="s">
-        <v>766</v>
+        <v>767</v>
       </c>
       <c r="B458" s="2" t="s">
         <v>123</v>
@@ -9486,12 +9521,12 @@
         <v>34</v>
       </c>
       <c r="D458" s="2" t="s">
-        <v>670</v>
+        <v>674</v>
       </c>
     </row>
     <row r="459" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A459" s="1" t="s">
-        <v>766</v>
+        <v>767</v>
       </c>
       <c r="B459" s="2" t="s">
         <v>123</v>
@@ -9500,15 +9535,12 @@
         <v>34</v>
       </c>
       <c r="D459" s="2" t="s">
-        <v>769</v>
-      </c>
-      <c r="G459" s="1" t="s">
-        <v>102</v>
+        <v>670</v>
       </c>
     </row>
     <row r="460" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A460" s="1" t="s">
-        <v>766</v>
+        <v>767</v>
       </c>
       <c r="B460" s="2" t="s">
         <v>123</v>
@@ -9525,7 +9557,7 @@
     </row>
     <row r="461" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A461" s="1" t="s">
-        <v>766</v>
+        <v>767</v>
       </c>
       <c r="B461" s="2" t="s">
         <v>123</v>
@@ -9542,7 +9574,7 @@
     </row>
     <row r="462" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A462" s="1" t="s">
-        <v>766</v>
+        <v>767</v>
       </c>
       <c r="B462" s="2" t="s">
         <v>123</v>
@@ -9551,12 +9583,15 @@
         <v>34</v>
       </c>
       <c r="D462" s="2" t="s">
-        <v>677</v>
+        <v>772</v>
+      </c>
+      <c r="G462" s="1" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="463" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A463" s="1" t="s">
-        <v>766</v>
+        <v>767</v>
       </c>
       <c r="B463" s="2" t="s">
         <v>123</v>
@@ -9565,15 +9600,12 @@
         <v>34</v>
       </c>
       <c r="D463" s="2" t="s">
-        <v>772</v>
-      </c>
-      <c r="G463" s="1" t="s">
-        <v>102</v>
+        <v>677</v>
       </c>
     </row>
     <row r="464" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A464" s="1" t="s">
-        <v>766</v>
+        <v>767</v>
       </c>
       <c r="B464" s="2" t="s">
         <v>123</v>
@@ -9590,35 +9622,35 @@
     </row>
     <row r="465" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A465" s="1" t="s">
+        <v>767</v>
+      </c>
+      <c r="B465" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="C465" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D465" s="2" t="s">
         <v>774</v>
       </c>
-      <c r="C465" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D465" s="2" t="s">
-        <v>775</v>
+      <c r="G465" s="1" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="466" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A466" s="1" t="s">
-        <v>774</v>
-      </c>
-      <c r="B466" s="2" t="s">
-        <v>123</v>
+        <v>775</v>
       </c>
       <c r="C466" s="1" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="D466" s="2" t="s">
         <v>776</v>
       </c>
-      <c r="H466" s="2" t="s">
-        <v>670</v>
-      </c>
     </row>
     <row r="467" s="3" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A467" s="1" t="s">
-        <v>774</v>
+        <v>775</v>
       </c>
       <c r="B467" s="2" t="s">
         <v>123</v>
@@ -9627,13 +9659,13 @@
         <v>34</v>
       </c>
       <c r="D467" s="2" t="s">
-        <v>672</v>
+        <v>777</v>
       </c>
       <c r="E467" s="0"/>
       <c r="F467" s="0"/>
       <c r="G467" s="0"/>
       <c r="H467" s="2" t="s">
-        <v>102</v>
+        <v>670</v>
       </c>
       <c r="I467" s="0"/>
       <c r="J467" s="0"/>
@@ -9655,7 +9687,7 @@
     </row>
     <row r="468" s="4" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A468" s="1" t="s">
-        <v>774</v>
+        <v>775</v>
       </c>
       <c r="B468" s="2" t="s">
         <v>123</v>
@@ -9664,12 +9696,14 @@
         <v>34</v>
       </c>
       <c r="D468" s="2" t="s">
-        <v>671</v>
+        <v>672</v>
       </c>
       <c r="E468" s="0"/>
       <c r="F468" s="0"/>
       <c r="G468" s="0"/>
-      <c r="H468" s="0"/>
+      <c r="H468" s="2" t="s">
+        <v>102</v>
+      </c>
       <c r="I468" s="0"/>
       <c r="J468" s="0"/>
       <c r="K468" s="0"/>
@@ -9690,7 +9724,7 @@
     </row>
     <row r="469" s="4" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A469" s="1" t="s">
-        <v>774</v>
+        <v>775</v>
       </c>
       <c r="B469" s="2" t="s">
         <v>123</v>
@@ -9699,7 +9733,7 @@
         <v>34</v>
       </c>
       <c r="D469" s="2" t="s">
-        <v>674</v>
+        <v>671</v>
       </c>
       <c r="E469" s="0"/>
       <c r="F469" s="0"/>
@@ -9725,7 +9759,7 @@
     </row>
     <row r="470" s="4" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A470" s="1" t="s">
-        <v>774</v>
+        <v>775</v>
       </c>
       <c r="B470" s="2" t="s">
         <v>123</v>
@@ -9734,7 +9768,7 @@
         <v>34</v>
       </c>
       <c r="D470" s="2" t="s">
-        <v>670</v>
+        <v>674</v>
       </c>
       <c r="E470" s="0"/>
       <c r="F470" s="0"/>
@@ -9760,14 +9794,16 @@
     </row>
     <row r="471" s="4" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A471" s="1" t="s">
-        <v>777</v>
-      </c>
-      <c r="B471" s="0"/>
+        <v>775</v>
+      </c>
+      <c r="B471" s="2" t="s">
+        <v>123</v>
+      </c>
       <c r="C471" s="1" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="D471" s="2" t="s">
-        <v>778</v>
+        <v>670</v>
       </c>
       <c r="E471" s="0"/>
       <c r="F471" s="0"/>
@@ -9793,14 +9829,14 @@
     </row>
     <row r="472" s="4" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A472" s="1" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
       <c r="B472" s="0"/>
       <c r="C472" s="1" t="s">
         <v>26</v>
       </c>
       <c r="D472" s="2" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="E472" s="0"/>
       <c r="F472" s="0"/>
@@ -9826,20 +9862,18 @@
     </row>
     <row r="473" s="4" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A473" s="1" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
       <c r="B473" s="0"/>
       <c r="C473" s="1" t="s">
         <v>26</v>
       </c>
       <c r="D473" s="2" t="s">
-        <v>591</v>
+        <v>781</v>
       </c>
       <c r="E473" s="0"/>
       <c r="F473" s="0"/>
-      <c r="G473" s="1" t="s">
-        <v>782</v>
-      </c>
+      <c r="G473" s="0"/>
       <c r="H473" s="0"/>
       <c r="I473" s="0"/>
       <c r="J473" s="0"/>
@@ -9859,6 +9893,41 @@
       <c r="X473" s="0"/>
       <c r="Y473" s="0"/>
     </row>
+    <row r="474" s="3" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A474" s="1" t="s">
+        <v>782</v>
+      </c>
+      <c r="B474" s="0"/>
+      <c r="C474" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D474" s="2" t="s">
+        <v>591</v>
+      </c>
+      <c r="E474" s="0"/>
+      <c r="F474" s="0"/>
+      <c r="G474" s="1" t="s">
+        <v>783</v>
+      </c>
+      <c r="H474" s="0"/>
+      <c r="I474" s="0"/>
+      <c r="J474" s="0"/>
+      <c r="K474" s="0"/>
+      <c r="L474" s="0"/>
+      <c r="M474" s="0"/>
+      <c r="N474" s="0"/>
+      <c r="O474" s="0"/>
+      <c r="P474" s="0"/>
+      <c r="Q474" s="0"/>
+      <c r="R474" s="0"/>
+      <c r="S474" s="0"/>
+      <c r="T474" s="0"/>
+      <c r="U474" s="0"/>
+      <c r="V474" s="0"/>
+      <c r="W474" s="0"/>
+      <c r="X474" s="0"/>
+      <c r="Y474" s="0"/>
+    </row>
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>

</xml_diff>

<commit_message>
[IMP] Temporary save 20220402
</commit_message>
<xml_diff>
--- a/clodoo/clodoo/transodoo.xlsx
+++ b/clodoo/clodoo/transodoo.xlsx
@@ -2766,9 +2766,9 @@
   <dimension ref="A1:AE1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="630" topLeftCell="N1" activePane="bottomLeft" state="split"/>
+      <pane xSplit="0" ySplit="630" topLeftCell="N181" activePane="bottomLeft" state="split"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="D10" activeCellId="0" sqref="D10"/>
+      <selection pane="bottomLeft" activeCell="G199" activeCellId="0" sqref="G199"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="27.01953125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2776,7 +2776,8 @@
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="27.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="7.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="28.92"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1021" min="4" style="1" width="27.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="28.93"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1021" min="5" style="1" width="27.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1023" style="2" width="9.14"/>
   </cols>
   <sheetData>

</xml_diff>